<commit_message>
Finalizado MAX2870. Compilado no testeado
</commit_message>
<xml_diff>
--- a/hardware/Pin definition Pocket Analyser.xlsx
+++ b/hardware/Pin definition Pocket Analyser.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adrie\Documents\00_Adriel\00_Proyectos\deFacultad\pocket-analyzer\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D1ACD05-5BC5-4A37-81A8-16C03F57C655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A12833-FD3A-40A0-8CED-DFE01D03D49F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{59E6B38B-99DD-4B5F-AB40-BFE77F10B5B7}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="100">
   <si>
     <t>Funcion</t>
   </si>
@@ -310,6 +310,33 @@
   </si>
   <si>
     <t>LED BLUE</t>
+  </si>
+  <si>
+    <t>MAX2871 - LD</t>
+  </si>
+  <si>
+    <t>MAX2871 - CE</t>
+  </si>
+  <si>
+    <t>MAX2871 - Rfenable</t>
+  </si>
+  <si>
+    <t>SWT-PA1</t>
+  </si>
+  <si>
+    <t>SWT-PA2</t>
+  </si>
+  <si>
+    <t>SWT-PB1</t>
+  </si>
+  <si>
+    <t>SWT-PB2</t>
+  </si>
+  <si>
+    <t>SWT-PC1</t>
+  </si>
+  <si>
+    <t>SWT-PC2</t>
   </si>
 </sst>
 </file>
@@ -818,7 +845,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1136,11 +1163,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8B9058C-A99F-49B8-9A33-A0DDA15A1DC1}">
   <dimension ref="B2:T40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="9.88671875" customWidth="1"/>
     <col min="4" max="4" width="11.77734375" customWidth="1"/>
@@ -1554,7 +1581,7 @@
         <v>7</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>26</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
@@ -1575,7 +1602,7 @@
         <v>8</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>26</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
@@ -1596,7 +1623,7 @@
         <v>9</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>26</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
@@ -1617,7 +1644,7 @@
         <v>10</v>
       </c>
       <c r="H19" s="17" t="s">
-        <v>26</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
@@ -1638,7 +1665,7 @@
         <v>11</v>
       </c>
       <c r="H20" s="17" t="s">
-        <v>26</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
@@ -1659,7 +1686,7 @@
         <v>12</v>
       </c>
       <c r="H21" s="17" t="s">
-        <v>26</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
@@ -1680,7 +1707,7 @@
         <v>13</v>
       </c>
       <c r="H22" s="17" t="s">
-        <v>26</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
@@ -1701,7 +1728,7 @@
         <v>14</v>
       </c>
       <c r="H23" s="17" t="s">
-        <v>26</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
@@ -1722,7 +1749,7 @@
         <v>15</v>
       </c>
       <c r="H24" s="17" t="s">
-        <v>26</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
@@ -2088,7 +2115,7 @@
       <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
@@ -2527,21 +2554,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E87C4DB29B667A4EA0E5F9AB0768AD03" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2e703ebf051f7a952c3f264e8bfbd6e2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="7fe592f4-80f8-4e02-8f41-a49f7dda7516" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5ab6c351620ec9c377910682c5cb4ff8" ns3:_="">
     <xsd:import namespace="7fe592f4-80f8-4e02-8f41-a49f7dda7516"/>
@@ -2691,31 +2703,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA2DDEA-4298-4F2F-80A1-B40952BE0F7B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="7fe592f4-80f8-4e02-8f41-a49f7dda7516"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C28E0058-2F99-4629-A836-C4E851D9B5B7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1ED71A87-E17B-411C-A1E1-AE9DD996E597}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2731,4 +2734,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C28E0058-2F99-4629-A836-C4E851D9B5B7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAA2DDEA-4298-4F2F-80A1-B40952BE0F7B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="7fe592f4-80f8-4e02-8f41-a49f7dda7516"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>